<commit_message>
organized strata_fee for payment distribution chart
</commit_message>
<xml_diff>
--- a/strata_fee_20230731.xlsx
+++ b/strata_fee_20230731.xlsx
@@ -8,24 +8,50 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0341E4FA-502E-4D05-BAF1-9746C309E72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBCFA9A-3F20-4195-A52B-F68455FA66D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlchart.v5.0" hidden="1">Sheet3!$J$1</definedName>
+    <definedName name="_xlchart.v5.1" hidden="1">Sheet3!$J$2:$J$66</definedName>
+    <definedName name="_xlchart.v5.10" hidden="1">Sheet3!#REF!</definedName>
+    <definedName name="_xlchart.v5.11" hidden="1">Sheet3!#REF!</definedName>
+    <definedName name="_xlchart.v5.2" hidden="1">Sheet3!$K$1</definedName>
+    <definedName name="_xlchart.v5.3" hidden="1">Sheet3!$K$2:$K$66</definedName>
+    <definedName name="_xlchart.v5.4" hidden="1">Sheet3!$L$1</definedName>
+    <definedName name="_xlchart.v5.5" hidden="1">Sheet3!$L$2:$L$66</definedName>
+    <definedName name="_xlchart.v5.6" hidden="1">Sheet3!#REF!</definedName>
+    <definedName name="_xlchart.v5.7" hidden="1">Sheet3!#REF!</definedName>
+    <definedName name="_xlchart.v5.8" hidden="1">Sheet3!#REF!</definedName>
+    <definedName name="_xlchart.v5.9" hidden="1">Sheet3!#REF!</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -253,6 +279,63 @@
   </si>
   <si>
     <t>20220527095424662054</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>fee_unit</t>
+  </si>
+  <si>
+    <t>payer</t>
+  </si>
+  <si>
+    <t>year-month</t>
+  </si>
+  <si>
+    <t>2022-10</t>
+  </si>
+  <si>
+    <t>2022-11</t>
+  </si>
+  <si>
+    <t>2022-12</t>
+  </si>
+  <si>
+    <t>2022-5</t>
+  </si>
+  <si>
+    <t>2022-6</t>
+  </si>
+  <si>
+    <t>2022-7</t>
+  </si>
+  <si>
+    <t>2022-8</t>
+  </si>
+  <si>
+    <t>2022-9</t>
+  </si>
+  <si>
+    <t>2023-1</t>
+  </si>
+  <si>
+    <t>2023-2</t>
+  </si>
+  <si>
+    <t>2023-3</t>
+  </si>
+  <si>
+    <t>2023-4</t>
+  </si>
+  <si>
+    <t>2023-5</t>
+  </si>
+  <si>
+    <t>2023-6</t>
+  </si>
+  <si>
+    <t>2023-7</t>
   </si>
 </sst>
 </file>
@@ -614,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1748,4 +1831,945 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01F659C-9D23-4E99-80EC-4C650027632E}">
+  <dimension ref="A1:D66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28">
+        <v>31</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31">
+        <v>31</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33">
+        <v>27</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47">
+        <v>29</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51">
+        <v>31</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54">
+        <v>31</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55">
+        <v>30</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56">
+        <v>29</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60">
+        <v>29</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61">
+        <v>29</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65">
+        <v>31</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66">
+        <v>27</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added slicer, exploring accumulation of fee_units
</commit_message>
<xml_diff>
--- a/strata_fee_20230731.xlsx
+++ b/strata_fee_20230731.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274EC875-84D0-4423-B67B-4C13BF20DB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21F4045-F4A8-45FD-8F6C-86D8E20EFB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="cleaned data" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet7" sheetId="8" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'cleaned data'!$A$1:$D$66</definedName>
+    <definedName name="Slicer_payer">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="39" r:id="rId4"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId5"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -40,8 +52,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -295,6 +329,9 @@
     <t>Jun</t>
   </si>
   <si>
+    <t>Jul</t>
+  </si>
+  <si>
     <t>Aug</t>
   </si>
   <si>
@@ -313,7 +350,19 @@
     <t>2023</t>
   </si>
   <si>
+    <t>Jan</t>
+  </si>
+  <si>
     <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>total_pays</t>
   </si>
 </sst>
 </file>
@@ -385,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -408,6 +457,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -677,6 +729,63 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -768,40 +877,96 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet7!$A$5:$A$15</c:f>
+              <c:f>Sheet7!$A$5:$A$33</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>02-Jun-22</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>01-Jul-22</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>01-Aug-22</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>01-Sep-22</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>02-Oct-22</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>01-Nov-22</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>01-Dec-22</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>02-Jan-23</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>01-Feb-23</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>01-Mar-23</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>01-Apr-23</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>01-May-23</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>01-Jul-23</c:v>
+                  </c:pt>
+                </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Jun</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>Jul</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>Aug</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>Sep</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>Oct</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>Nov</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>Dec</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
                     <c:v>Feb</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="9">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Jul</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>2022</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>2023</c:v>
                   </c:pt>
                 </c:lvl>
@@ -810,12 +975,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet7!$B$5:$B$15</c:f>
+              <c:f>Sheet7!$B$5:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -830,13 +995,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,16 +1857,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>746760</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1711,13 +1891,91 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>708660</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>39189</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>98244</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="payer">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8829B32-68AC-8930-1961-390197A1C322}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="payer"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2948940" y="222069"/>
+              <a:ext cx="1828800" cy="2436495"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dongli" refreshedDate="45138.522558564815" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="65" xr:uid="{865697DA-7FBF-4A30-AEC2-F06A1A95E045}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C66" sheet="cleaned data"/>
+    <worksheetSource ref="A1:B66" sheet="cleaned data"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Date" numFmtId="15">
@@ -1832,7 +2090,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="1917614629"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -2170,7 +2428,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12F9B551-ABA9-4908-A502-1E5BED92D63A}" name="PivotTable23" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A4:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="A4:B33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="15" showAll="0">
       <items count="44">
@@ -2240,20 +2498,20 @@
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="15">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2270,10 +2528,10 @@
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
-        <item sd="0" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item sd="0" x="3"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2283,36 +2541,90 @@
     <field x="3"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="29">
     <i>
       <x v="1"/>
     </i>
     <i r="1">
       <x v="6"/>
     </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
     <i r="1">
       <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
     </i>
     <i r="1">
       <x v="9"/>
     </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
     <i r="1">
       <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
     </i>
     <i r="1">
       <x v="11"/>
     </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
     <i r="1">
       <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i r="1">
       <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="34"/>
     </i>
     <i r="1">
       <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="40"/>
     </i>
     <i t="grand">
       <x/>
@@ -2322,7 +2634,7 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="2" item="2" hier="-1"/>
+    <pageField fld="2" item="4" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of fee_unit" fld="1" baseField="0" baseItem="0"/>
@@ -2348,6 +2660,31 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_payer" xr10:uid="{12A1E9C4-3B82-4A89-B4FE-5184519D0C73}" sourceName="payer">
+  <pivotTables>
+    <pivotTable tabId="8" name="PivotTable23"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1917614629">
+      <items count="5">
+        <i x="0"/>
+        <i x="1"/>
+        <i x="4"/>
+        <i x="3"/>
+        <i x="2" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="payer" xr10:uid="{BF45FBC2-BB81-41DF-9B10-98B5738A3CF8}" cache="Slicer_payer" caption="payer" rowHeight="234950"/>
+</slicers>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3753,763 +4090,1022 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7BACAC-EFC0-4D7F-A488-F4B660678DD6}">
-  <dimension ref="A1:C66"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="10">
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11">
+        <v>44708</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2:D66">INDEX($B$2:$C$66,MAX(IF($A$2:$A$66=$E$1,ROW($A$2:$A$66)-ROW(INDEX($A$2:$A$66,1,1))+1)), 2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1">
+      <c r="A3" s="11">
+        <v>44712</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1">
+      <c r="A4" s="11">
+        <v>44714</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1">
+      <c r="A5" s="11">
+        <v>44715</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1">
+      <c r="A6" s="11">
+        <v>44715</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1">
+      <c r="A7" s="11">
+        <v>44741</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="11">
+        <v>44741</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1">
+      <c r="A9" s="11">
+        <v>44742</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1">
+      <c r="A10" s="11">
+        <v>44743</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1">
+      <c r="A11" s="11">
+        <v>44743</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="11">
+        <v>44771</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f>E8+D12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1">
+      <c r="A13" s="11">
+        <v>44772</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" hidden="1">
+      <c r="A14" s="11">
+        <v>44773</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1">
+      <c r="A15" s="11">
+        <v>44774</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1">
+      <c r="A16" s="11">
+        <v>44774</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="11">
+        <v>44804</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f>E12+D17</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1">
+      <c r="A18" s="11">
+        <v>44805</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1">
+      <c r="A19" s="11">
+        <v>44805</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1">
+      <c r="A20" s="11">
+        <v>44813</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1">
+      <c r="A21" s="11">
+        <v>44833</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1">
+      <c r="A22" s="11">
+        <v>44834</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1">
+      <c r="A23" s="11">
+        <v>44836</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="11">
+        <v>44836</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" hidden="1">
+      <c r="A25" s="11">
+        <v>44838</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1">
+      <c r="A26" s="11">
+        <v>44862</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1">
+      <c r="A27" s="11">
+        <v>44866</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1">
+      <c r="A28" s="11">
+        <v>44866</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="11">
+        <v>44866</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" hidden="1">
+      <c r="A30" s="11">
+        <v>44879</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1">
+      <c r="A31" s="11">
+        <v>44896</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1">
+      <c r="A32" s="11">
+        <v>44896</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="11">
+        <v>44900</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f>E29+D33</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1">
+      <c r="A34" s="11">
+        <v>44900</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1">
+      <c r="A35" s="11">
+        <v>44922</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" hidden="1">
+      <c r="A36" s="11">
+        <v>44922</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1">
+      <c r="A37" s="11">
+        <v>44926</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="11">
+        <v>44927</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1">
+      <c r="A39" s="11">
+        <v>44928</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1">
+      <c r="A40" s="11">
+        <v>44957</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1">
+      <c r="A41" s="11">
+        <v>44958</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1">
+      <c r="A42" s="11">
+        <v>44958</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="11">
+        <v>44958</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1">
+      <c r="A44" s="11">
+        <v>44981</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1">
+      <c r="A45" s="11">
+        <v>44986</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1">
+      <c r="A46" s="11">
+        <v>44986</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="11">
+        <v>44987</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f>E43+D47</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1">
+      <c r="A48" s="11">
+        <v>44987</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1">
+      <c r="A49" s="11">
+        <v>44987</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="11">
+        <v>45015</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1">
+      <c r="A51" s="11">
+        <v>45016</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1">
+      <c r="A52" s="11">
+        <v>45016</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1">
+      <c r="A53" s="11">
+        <v>45017</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" hidden="1">
+      <c r="A54" s="11">
+        <v>45044</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1">
+      <c r="A55" s="11">
+        <v>45047</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="11">
+        <v>45047</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" hidden="1">
+      <c r="A57" s="11">
+        <v>45047</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" hidden="1">
+      <c r="A58" s="11">
+        <v>45047</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" hidden="1">
+      <c r="A59" s="11">
+        <v>45047</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" hidden="1">
+      <c r="A60" s="11">
+        <v>45047</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" hidden="1">
+      <c r="A61" s="11">
+        <v>45076</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="11">
+        <v>45083</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" hidden="1">
+      <c r="A63" s="11">
+        <v>45107</v>
+      </c>
+      <c r="B63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" hidden="1">
+      <c r="A64" s="11">
+        <v>45108</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" hidden="1">
+      <c r="A65" s="11">
+        <v>45111</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="11">
         <v>45112</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="10">
-        <v>45111</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="10">
-        <v>45108</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="10">
-        <v>45107</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="10">
-        <v>45083</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="10">
-        <v>45076</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="10">
-        <v>45047</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="10">
-        <v>45047</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="10">
-        <v>45047</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="10">
-        <v>45047</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="10">
-        <v>45047</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="10">
-        <v>45047</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="10">
-        <v>45044</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="10">
-        <v>45017</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="10">
-        <v>45016</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="10">
-        <v>45016</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="10">
-        <v>45015</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="10">
-        <v>44987</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="10">
-        <v>44987</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="10">
-        <v>44987</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="10">
-        <v>44986</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="10">
-        <v>44986</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="10">
-        <v>44981</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="10">
-        <v>44958</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="10">
-        <v>44958</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="10">
-        <v>44958</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="10">
-        <v>44957</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="10">
-        <v>44928</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="10">
-        <v>44927</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="10">
-        <v>44926</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="10">
-        <v>44922</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="10">
-        <v>44922</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="10">
-        <v>44900</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="10">
-        <v>44900</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="10">
-        <v>44896</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="10">
-        <v>44896</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="10">
-        <v>44879</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="10">
-        <v>44866</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="10">
-        <v>44866</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="10">
-        <v>44866</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="10">
-        <v>44862</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="10">
-        <v>44838</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="10">
-        <v>44836</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="10">
-        <v>44836</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="10">
-        <v>44834</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="10">
-        <v>44833</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="10">
-        <v>44813</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="10">
-        <v>44805</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="10">
-        <v>44805</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="10">
-        <v>44804</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="10">
-        <v>44774</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="10">
-        <v>44774</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="10">
-        <v>44773</v>
-      </c>
-      <c r="B54">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="10">
-        <v>44772</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="10">
-        <v>44771</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="10">
-        <v>44743</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="10">
-        <v>44743</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="10">
-        <v>44742</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="10">
-        <v>44741</v>
-      </c>
-      <c r="B60">
-        <v>2</v>
-      </c>
-      <c r="C60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="10">
-        <v>44741</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="10">
-        <v>44715</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="10">
-        <v>44715</v>
-      </c>
-      <c r="B63">
-        <v>2</v>
-      </c>
-      <c r="C63" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="10">
-        <v>44714</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="10">
-        <v>44712</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="10">
-        <v>44708</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <f>E62+D66</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D66" xr:uid="{DC7BACAC-EFC0-4D7F-A488-F4B660678DD6}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="DONGLI LIU"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D66">
+    <sortCondition ref="A1:A66"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B089A-5F14-499D-895B-7DCA63C7442F}">
-  <dimension ref="A2:B15"/>
+  <dimension ref="A2:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4519,7 +5115,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4535,7 +5131,7 @@
         <v>81</v>
       </c>
       <c r="B5" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4543,12 +5139,12 @@
         <v>83</v>
       </c>
       <c r="B6" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8" t="s">
-        <v>84</v>
+      <c r="A7" s="10">
+        <v>44714</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -4556,15 +5152,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8" t="s">
-        <v>86</v>
+      <c r="A9" s="10">
+        <v>44743</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -4572,31 +5168,31 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="8" t="s">
-        <v>88</v>
+      <c r="A11" s="10">
+        <v>44774</v>
       </c>
       <c r="B11" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="7" t="s">
-        <v>89</v>
+      <c r="A12" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B12" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="8" t="s">
-        <v>90</v>
+      <c r="A13" s="10">
+        <v>44805</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
@@ -4604,22 +5200,173 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="10">
+        <v>44836</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="10">
+        <v>44866</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10">
+        <v>44896</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="10">
+        <v>44928</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="10">
+        <v>44958</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="10">
+        <v>44986</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="10">
+        <v>45017</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="7" t="s">
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="10">
+        <v>45047</v>
+      </c>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="10">
+        <v>45108</v>
+      </c>
+      <c r="B32" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="9">
-        <v>12</v>
+      <c r="B33" s="9">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added total paid_units per payer chart
</commit_message>
<xml_diff>
--- a/strata_fee_20230731.xlsx
+++ b/strata_fee_20230731.xlsx
@@ -8,29 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFF6100-C125-43BE-9177-4AA32B36E3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7EF70B-B8F2-4858-8C73-32C19AD9964F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="cleaned data" sheetId="6" r:id="rId2"/>
-    <sheet name="pivot 2" sheetId="9" r:id="rId3"/>
-    <sheet name="pivot" sheetId="8" r:id="rId4"/>
+    <sheet name="pivot" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'cleaned data'!$A$1:$C$66</definedName>
-    <definedName name="Slicer_payer1">#N/A</definedName>
+    <definedName name="Slicer_payer">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId5"/>
-    <pivotCache cacheId="17" r:id="rId6"/>
+    <pivotCache cacheId="18" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId7"/>
+        <x14:slicerCache r:id="rId5"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -55,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -334,9 +332,6 @@
   </si>
   <si>
     <t>Mar</t>
-  </si>
-  <si>
-    <t>units paid</t>
   </si>
   <si>
     <t>EDWIN ALBERT IMHOFF</t>
@@ -429,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -450,9 +445,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -477,797 +469,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[strata_fee_20230731.xlsx]pivot 2!PivotTable1</c:name>
-    <c:fmtId val="0"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-CA"/>
-              <a:t>Strata</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Fee Payment History</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="inEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="t"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="-3.3333333333333333E-2"/>
-              <c:y val="-2.8070175438596492E-2"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="3"/>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="4"/>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="5"/>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'pivot 2'!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'pivot 2'!$A$4:$A$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="1"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>31-Jul-23</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Jul</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2023</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'pivot 2'!$B$4:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4911-46E6-ACD4-4640D99352A9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:axId val="2042008751"/>
-        <c:axId val="2042001071"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2042008751"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2042001071"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2042001071"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-CA"/>
-                  <a:t>Fee Unit ( $150 /unit )</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2042008751"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2108,6 +1309,498 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[strata_fee_20230731.xlsx]pivot!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivot!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>pivot!$A$25:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>SIDDHARTH SINHA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>XIAOPENG FENG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DONGLI LIU</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TRACY CARRIER</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>EDWIN ALBERT IMHOFF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivot!$B$25:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C2E5-4824-9E49-3C6FDE39A80B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1329728272"/>
+        <c:axId val="713974208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1329728272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="713974208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="713974208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1329728272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3266,23 +2959,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>479367</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>105988</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>334587</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>90748</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{304F66F2-D424-E780-1274-0390748187EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A1FB961-C1CE-B923-44A8-D934A713B8AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3300,27 +2993,63 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{354D1546-BFA7-6F95-4A0F-6175D4A8590A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>602772</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1484</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>602772</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>62716</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>89535</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="payer 1">
+            <xdr:cNvPr id="5" name="payer">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17209CEE-E95D-3F99-A99D-515442BC0D6D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{782B7932-C661-FF69-CEF3-65B1AE1B2E2F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3332,12 +3061,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="payer 1"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="payer"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3347,8 +3076,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7308372" y="1794425"/>
-              <a:ext cx="1828800" cy="2392056"/>
+              <a:off x="8313420" y="4206240"/>
+              <a:ext cx="1828800" cy="2466975"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3381,173 +3110,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>746760</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A1FB961-C1CE-B923-44A8-D934A713B8AB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dongli" refreshedDate="45142.920207870367" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="65" xr:uid="{52ED5432-E891-4F20-ABDB-0FEFE682FF87}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C66" sheet="cleaned data"/>
-  </cacheSource>
-  <cacheFields count="6">
-    <cacheField name="Date" numFmtId="15">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2022-05-27T00:00:00" maxDate="2023-08-03T00:00:00" count="47">
-        <d v="2022-05-27T00:00:00"/>
-        <d v="2022-06-29T00:00:00"/>
-        <d v="2022-07-29T00:00:00"/>
-        <d v="2022-08-31T00:00:00"/>
-        <d v="2022-10-02T00:00:00"/>
-        <d v="2022-11-01T00:00:00"/>
-        <d v="2022-12-05T00:00:00"/>
-        <d v="2023-01-01T00:00:00"/>
-        <d v="2023-02-01T00:00:00"/>
-        <d v="2023-03-02T00:00:00"/>
-        <d v="2023-03-30T00:00:00"/>
-        <d v="2023-05-01T00:00:00"/>
-        <d v="2023-06-06T00:00:00"/>
-        <d v="2023-07-05T00:00:00"/>
-        <d v="2023-08-02T00:00:00"/>
-        <d v="2023-07-31T00:00:00"/>
-        <d v="2022-06-03T00:00:00"/>
-        <d v="2022-07-31T00:00:00"/>
-        <d v="2022-09-29T00:00:00"/>
-        <d v="2023-03-31T00:00:00"/>
-        <d v="2023-07-04T00:00:00"/>
-        <d v="2022-06-30T00:00:00"/>
-        <d v="2022-08-01T00:00:00"/>
-        <d v="2022-09-09T00:00:00"/>
-        <d v="2022-10-04T00:00:00"/>
-        <d v="2022-11-14T00:00:00"/>
-        <d v="2022-12-27T00:00:00"/>
-        <d v="2023-02-24T00:00:00"/>
-        <d v="2023-07-26T00:00:00"/>
-        <d v="2022-05-31T00:00:00"/>
-        <d v="2022-07-01T00:00:00"/>
-        <d v="2022-07-30T00:00:00"/>
-        <d v="2022-09-01T00:00:00"/>
-        <d v="2022-09-30T00:00:00"/>
-        <d v="2022-10-28T00:00:00"/>
-        <d v="2022-12-01T00:00:00"/>
-        <d v="2022-12-31T00:00:00"/>
-        <d v="2023-01-31T00:00:00"/>
-        <d v="2023-03-01T00:00:00"/>
-        <d v="2023-04-28T00:00:00"/>
-        <d v="2023-05-30T00:00:00"/>
-        <d v="2023-06-30T00:00:00"/>
-        <d v="2023-07-28T00:00:00"/>
-        <d v="2022-06-02T00:00:00"/>
-        <d v="2023-01-02T00:00:00"/>
-        <d v="2023-07-01T00:00:00" u="1"/>
-        <d v="2023-04-01T00:00:00" u="1"/>
-      </sharedItems>
-      <fieldGroup par="5"/>
-    </cacheField>
-    <cacheField name="payer" numFmtId="0">
-      <sharedItems count="6">
-        <s v="DONGLI LIU"/>
-        <s v="EDWIN ALBERT IMHOFF"/>
-        <s v="EDWINALBERT IMHOFF"/>
-        <s v="SIDDHARTH SINHA"/>
-        <s v="TRACY CARRIER"/>
-        <s v="XIAOPENG FENG"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="fee_unit" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
-    </cacheField>
-    <cacheField name="Months (Date)" numFmtId="0" databaseField="0">
-      <fieldGroup base="0">
-        <rangePr groupBy="months" startDate="2022-05-27T00:00:00" endDate="2023-08-03T00:00:00"/>
-        <groupItems count="14">
-          <s v="&lt;2022-05-27"/>
-          <s v="Jan"/>
-          <s v="Feb"/>
-          <s v="Mar"/>
-          <s v="Apr"/>
-          <s v="May"/>
-          <s v="Jun"/>
-          <s v="Jul"/>
-          <s v="Aug"/>
-          <s v="Sep"/>
-          <s v="Oct"/>
-          <s v="Nov"/>
-          <s v="Dec"/>
-          <s v="&gt;2023-08-03"/>
-        </groupItems>
-      </fieldGroup>
-    </cacheField>
-    <cacheField name="Quarters (Date)" numFmtId="0" databaseField="0">
-      <fieldGroup base="0">
-        <rangePr groupBy="quarters" startDate="2022-05-27T00:00:00" endDate="2023-08-03T00:00:00"/>
-        <groupItems count="6">
-          <s v="&lt;2022-05-27"/>
-          <s v="Qtr1"/>
-          <s v="Qtr2"/>
-          <s v="Qtr3"/>
-          <s v="Qtr4"/>
-          <s v="&gt;2023-08-03"/>
-        </groupItems>
-      </fieldGroup>
-    </cacheField>
-    <cacheField name="Years (Date)" numFmtId="0" databaseField="0">
-      <fieldGroup base="0">
-        <rangePr groupBy="years" startDate="2022-05-27T00:00:00" endDate="2023-08-03T00:00:00"/>
-        <groupItems count="4">
-          <s v="&lt;2022-05-27"/>
-          <s v="2022"/>
-          <s v="2023"/>
-          <s v="&gt;2023-08-03"/>
-        </groupItems>
-      </fieldGroup>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition pivotCacheId="2142732816"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dongli" refreshedDate="45142.922907638887" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="71" xr:uid="{CFDD7A6A-69B9-4348-91AC-64659B55C3AB}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:C72" sheet="cleaned data"/>
@@ -3670,343 +3233,13 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="2056893067"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="65">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="12"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="1"/>
-    <n v="10"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="17"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="2"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <x v="2"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <x v="2"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <x v="2"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="22"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="23"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="24"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="25"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="26"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="26"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="27"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="28"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="28"/>
-    <x v="3"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="30"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="32"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="33"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="34"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="35"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="36"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="37"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="38"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="39"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="40"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="41"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="42"/>
-    <x v="4"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="43"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="30"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="22"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="32"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="35"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="44"/>
-    <x v="5"/>
-    <n v="1"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="71">
   <r>
     <x v="0"/>
@@ -4367,10 +3600,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62D6A957-B10E-4FCD-B1F3-555C111C3610}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{915D806B-8927-47A8-8343-DEA578A58961}" name="PivotTable1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+  <location ref="A24:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
-    <pivotField axis="axisRow" numFmtId="15" showAll="0">
+    <pivotField numFmtId="15" showAll="0">
       <items count="48">
         <item x="0"/>
         <item x="29"/>
@@ -4406,88 +3639,71 @@
         <item x="9"/>
         <item x="10"/>
         <item x="19"/>
-        <item m="1" x="46"/>
+        <item x="45"/>
         <item x="39"/>
         <item x="11"/>
         <item x="40"/>
         <item x="12"/>
         <item x="41"/>
-        <item m="1" x="45"/>
+        <item x="46"/>
         <item x="20"/>
         <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
         <item x="28"/>
         <item x="42"/>
+        <item x="15"/>
+        <item x="14"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
-        <item h="1" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item sd="0" x="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="6">
+        <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item sd="0" x="13"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item sd="0" x="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="3">
-    <field x="5"/>
-    <field x="3"/>
-    <field x="0"/>
+  <rowFields count="1">
+    <field x="1"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="6">
     <i>
       <x v="2"/>
     </i>
-    <i r="1">
-      <x v="7"/>
+    <i>
+      <x v="4"/>
     </i>
-    <i r="2">
-      <x v="44"/>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -4497,7 +3713,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="units paid" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Sum of fee_unit" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="0" series="1">
@@ -4523,7 +3739,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5709480-1479-4DD6-B514-8C458752D08E}" name="PivotTable23" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5709480-1479-4DD6-B514-8C458752D08E}" name="PivotTable23" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A4:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField numFmtId="15" showAll="0">
@@ -4727,19 +3943,18 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_payer1" xr10:uid="{1F403C8E-07AC-42EC-9C37-0EF48B9896CE}" sourceName="payer">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_payer" xr10:uid="{1F15D377-5226-4333-9E89-A205101AC46F}" sourceName="payer">
   <pivotTables>
-    <pivotTable tabId="9" name="PivotTable1"/>
+    <pivotTable tabId="8" name="PivotTable1"/>
   </pivotTables>
   <data>
-    <tabular pivotCacheId="2142732816">
-      <items count="6">
-        <i x="0"/>
+    <tabular pivotCacheId="2056893067">
+      <items count="5">
+        <i x="0" s="1"/>
         <i x="1" s="1"/>
-        <i x="2"/>
-        <i x="3"/>
-        <i x="4"/>
-        <i x="5"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
       </items>
     </tabular>
   </data>
@@ -4748,7 +3963,7 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="payer 1" xr10:uid="{D7BE1EFC-097E-43AF-A2CB-43230A75BA99}" cache="Slicer_payer1" caption="payer" rowHeight="234950"/>
+  <slicer name="payer" xr10:uid="{1D1F71E3-701E-4214-9249-E6BB59BF0CA4}" cache="Slicer_payer" caption="payer" rowHeight="234950"/>
 </slicers>
 </file>
 
@@ -5055,7 +4270,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -5072,7 +4287,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -5089,10 +4304,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5106,7 +4321,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -5123,7 +4338,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -5140,7 +4355,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -6261,8 +5476,8 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6284,7 +5499,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>44708</v>
       </c>
       <c r="B2" t="s">
@@ -6295,7 +5510,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>44741</v>
       </c>
       <c r="B3" t="s">
@@ -6306,7 +5521,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>44771</v>
       </c>
       <c r="B4" t="s">
@@ -6317,7 +5532,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>44804</v>
       </c>
       <c r="B5" t="s">
@@ -6328,7 +5543,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>44836</v>
       </c>
       <c r="B6" t="s">
@@ -6339,7 +5554,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>44866</v>
       </c>
       <c r="B7" t="s">
@@ -6350,7 +5565,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>44900</v>
       </c>
       <c r="B8" t="s">
@@ -6361,7 +5576,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>44927</v>
       </c>
       <c r="B9" t="s">
@@ -6372,7 +5587,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>44958</v>
       </c>
       <c r="B10" t="s">
@@ -6383,7 +5598,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>44987</v>
       </c>
       <c r="B11" t="s">
@@ -6394,7 +5609,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>45015</v>
       </c>
       <c r="B12" t="s">
@@ -6405,7 +5620,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>45047</v>
       </c>
       <c r="B13" t="s">
@@ -6416,7 +5631,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>45083</v>
       </c>
       <c r="B14" t="s">
@@ -6427,7 +5642,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>45112</v>
       </c>
       <c r="B15" t="s">
@@ -6438,7 +5653,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>45140</v>
       </c>
       <c r="B16" t="s">
@@ -6447,154 +5662,154 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="10">
-        <v>45138</v>
+      <c r="A17" s="9">
+        <v>44715</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="E17" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="10">
-        <v>44715</v>
+      <c r="A18" s="9">
+        <v>44741</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="10">
-        <v>44741</v>
+      <c r="A19" s="9">
+        <v>44773</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="10">
-        <v>44773</v>
+      <c r="A20" s="9">
+        <v>44833</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="9">
+        <v>44866</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="10">
-        <v>44833</v>
-      </c>
-      <c r="B21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-    </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="10">
-        <v>44866</v>
+      <c r="A22" s="9">
+        <v>44900</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="10">
-        <v>44900</v>
+      <c r="A23" s="9">
+        <v>44958</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="10">
-        <v>44958</v>
+      <c r="A24" s="9">
+        <v>44987</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="9">
+        <v>44987</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="9">
+        <v>45016</v>
+      </c>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="10">
-        <v>44987</v>
-      </c>
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="10">
-        <v>44987</v>
-      </c>
-      <c r="B26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="10">
-        <v>45016</v>
+      <c r="A27" s="9">
+        <v>45047</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="10">
-        <v>45047</v>
+      <c r="A28" s="9">
+        <v>45111</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="10">
-        <v>45111</v>
+      <c r="A29" s="9">
+        <v>45138</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>44715</v>
       </c>
       <c r="B30" t="s">
@@ -6605,7 +5820,7 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="10">
+      <c r="A31" s="9">
         <v>44742</v>
       </c>
       <c r="B31" t="s">
@@ -6616,7 +5831,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="10">
+      <c r="A32" s="9">
         <v>44774</v>
       </c>
       <c r="B32" t="s">
@@ -6627,7 +5842,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>44813</v>
       </c>
       <c r="B33" t="s">
@@ -6638,7 +5853,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <v>44838</v>
       </c>
       <c r="B34" t="s">
@@ -6649,7 +5864,7 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="10">
+      <c r="A35" s="9">
         <v>44879</v>
       </c>
       <c r="B35" t="s">
@@ -6660,7 +5875,7 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="10">
+      <c r="A36" s="9">
         <v>44922</v>
       </c>
       <c r="B36" t="s">
@@ -6671,7 +5886,7 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <v>44922</v>
       </c>
       <c r="B37" t="s">
@@ -6682,7 +5897,7 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="10">
+      <c r="A38" s="9">
         <v>44981</v>
       </c>
       <c r="B38" t="s">
@@ -6693,7 +5908,7 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="10">
+      <c r="A39" s="9">
         <v>45047</v>
       </c>
       <c r="B39" t="s">
@@ -6704,7 +5919,7 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="10">
+      <c r="A40" s="9">
         <v>45047</v>
       </c>
       <c r="B40" t="s">
@@ -6715,7 +5930,7 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="10">
+      <c r="A41" s="9">
         <v>45047</v>
       </c>
       <c r="B41" t="s">
@@ -6726,7 +5941,7 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="10">
+      <c r="A42" s="9">
         <v>45133</v>
       </c>
       <c r="B42" t="s">
@@ -6735,10 +5950,10 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="E42" s="11"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="10">
+      <c r="A43" s="9">
         <v>45133</v>
       </c>
       <c r="B43" t="s">
@@ -6747,10 +5962,10 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="E43" s="11"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="10">
+      <c r="A44" s="9">
         <v>44712</v>
       </c>
       <c r="B44" t="s">
@@ -6761,7 +5976,7 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="10">
+      <c r="A45" s="9">
         <v>44743</v>
       </c>
       <c r="B45" t="s">
@@ -6772,7 +5987,7 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="10">
+      <c r="A46" s="9">
         <v>44772</v>
       </c>
       <c r="B46" t="s">
@@ -6783,7 +5998,7 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="10">
+      <c r="A47" s="9">
         <v>44805</v>
       </c>
       <c r="B47" t="s">
@@ -6794,7 +6009,7 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="10">
+      <c r="A48" s="9">
         <v>44834</v>
       </c>
       <c r="B48" t="s">
@@ -6805,7 +6020,7 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="10">
+      <c r="A49" s="9">
         <v>44862</v>
       </c>
       <c r="B49" t="s">
@@ -6816,7 +6031,7 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="10">
+      <c r="A50" s="9">
         <v>44896</v>
       </c>
       <c r="B50" t="s">
@@ -6827,7 +6042,7 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="10">
+      <c r="A51" s="9">
         <v>44926</v>
       </c>
       <c r="B51" t="s">
@@ -6838,7 +6053,7 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="10">
+      <c r="A52" s="9">
         <v>44957</v>
       </c>
       <c r="B52" t="s">
@@ -6849,7 +6064,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="10">
+      <c r="A53" s="9">
         <v>44986</v>
       </c>
       <c r="B53" t="s">
@@ -6860,7 +6075,7 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="10">
+      <c r="A54" s="9">
         <v>45016</v>
       </c>
       <c r="B54" t="s">
@@ -6871,7 +6086,7 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="10">
+      <c r="A55" s="9">
         <v>45044</v>
       </c>
       <c r="B55" t="s">
@@ -6882,7 +6097,7 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="10">
+      <c r="A56" s="9">
         <v>45076</v>
       </c>
       <c r="B56" t="s">
@@ -6893,7 +6108,7 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="10">
+      <c r="A57" s="9">
         <v>45107</v>
       </c>
       <c r="B57" t="s">
@@ -6904,7 +6119,7 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="10">
+      <c r="A58" s="9">
         <v>45135</v>
       </c>
       <c r="B58" t="s">
@@ -6913,10 +6128,10 @@
       <c r="C58">
         <v>1</v>
       </c>
-      <c r="E58" s="11"/>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="10">
+      <c r="A59" s="9">
         <v>44714</v>
       </c>
       <c r="B59" t="s">
@@ -6927,7 +6142,7 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="10">
+      <c r="A60" s="9">
         <v>44743</v>
       </c>
       <c r="B60" t="s">
@@ -6938,7 +6153,7 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="10">
+      <c r="A61" s="9">
         <v>44774</v>
       </c>
       <c r="B61" t="s">
@@ -6949,7 +6164,7 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="10">
+      <c r="A62" s="9">
         <v>44805</v>
       </c>
       <c r="B62" t="s">
@@ -6960,7 +6175,7 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="10">
+      <c r="A63" s="9">
         <v>44836</v>
       </c>
       <c r="B63" t="s">
@@ -6971,7 +6186,7 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="10">
+      <c r="A64" s="9">
         <v>44866</v>
       </c>
       <c r="B64" t="s">
@@ -6982,7 +6197,7 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="10">
+      <c r="A65" s="9">
         <v>44896</v>
       </c>
       <c r="B65" t="s">
@@ -6993,7 +6208,7 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="10">
+      <c r="A66" s="9">
         <v>44928</v>
       </c>
       <c r="B66" t="s">
@@ -7004,7 +6219,7 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="10">
+      <c r="A67" s="9">
         <v>44958</v>
       </c>
       <c r="B67" t="s">
@@ -7015,7 +6230,7 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="10">
+      <c r="A68" s="9">
         <v>44986</v>
       </c>
       <c r="B68" t="s">
@@ -7026,7 +6241,7 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="10">
+      <c r="A69" s="9">
         <v>45017</v>
       </c>
       <c r="B69" t="s">
@@ -7037,7 +6252,7 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="10">
+      <c r="A70" s="9">
         <v>45047</v>
       </c>
       <c r="B70" t="s">
@@ -7048,7 +6263,7 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="10">
+      <c r="A71" s="9">
         <v>45108</v>
       </c>
       <c r="B71" t="s">
@@ -7059,7 +6274,7 @@
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="10">
+      <c r="A72" s="9">
         <v>45140</v>
       </c>
       <c r="B72" t="s">
@@ -7068,7 +6283,7 @@
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="E72" s="11"/>
+      <c r="E72" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C66" xr:uid="{DC7BACAC-EFC0-4D7F-A488-F4B660678DD6}">
@@ -7076,92 +6291,25 @@
       <sortCondition ref="A1:A66"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E74">
-    <sortCondition ref="B2:B74"/>
-    <sortCondition ref="A2:A74"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C72">
+    <sortCondition ref="B2:B72"/>
+    <sortCondition ref="A2:A72"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A41D512-AE0C-4D49-8861-E8FDA56B98CF}">
-  <dimension ref="A3:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B089A-5F14-499D-895B-7DCA63C7442F}">
+  <dimension ref="A2:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="I13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB32" sqref="AB32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="9">
-        <v>45138</v>
-      </c>
-      <c r="B6" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="12">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
-      <x14:slicerList>
-        <x14:slicer r:id="rId3"/>
-      </x14:slicerList>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B089A-5F14-499D-895B-7DCA63C7442F}">
-  <dimension ref="A2:B21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
@@ -7188,7 +6336,7 @@
       <c r="A5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>7</v>
       </c>
     </row>
@@ -7196,7 +6344,7 @@
       <c r="A6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7204,7 +6352,7 @@
       <c r="A7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7212,7 +6360,7 @@
       <c r="A8" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7220,7 +6368,7 @@
       <c r="A9" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7228,7 +6376,7 @@
       <c r="A10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7236,7 +6384,7 @@
       <c r="A11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7244,7 +6392,7 @@
       <c r="A12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7252,7 +6400,7 @@
       <c r="A13" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>8</v>
       </c>
     </row>
@@ -7260,7 +6408,7 @@
       <c r="A14" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7268,7 +6416,7 @@
       <c r="A15" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7276,7 +6424,7 @@
       <c r="A16" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>2</v>
       </c>
     </row>
@@ -7284,7 +6432,7 @@
       <c r="A17" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7292,7 +6440,7 @@
       <c r="A18" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7300,7 +6448,7 @@
       <c r="A19" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7308,7 +6456,7 @@
       <c r="A20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="11">
         <v>1</v>
       </c>
     </row>
@@ -7316,12 +6464,75 @@
       <c r="A21" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="11">
         <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="11">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
optimized day display in strata_fee distribution
</commit_message>
<xml_diff>
--- a/strata_fee_20230731.xlsx
+++ b/strata_fee_20230731.xlsx
@@ -8,27 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7EF70B-B8F2-4858-8C73-32C19AD9964F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9318C0-599F-4F39-82ED-151D85580772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="cleaned data" sheetId="6" r:id="rId2"/>
     <sheet name="pivot" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'cleaned data'!$A$1:$C$66</definedName>
     <definedName name="Slicer_payer">#N/A</definedName>
+    <definedName name="Slicer_payer1">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId4"/>
+    <pivotCache cacheId="18" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId5"/>
+        <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -53,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -332,6 +335,12 @@
   </si>
   <si>
     <t>Mar</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Apr</t>
   </si>
   <si>
     <t>EDWIN ALBERT IMHOFF</t>
@@ -359,8 +368,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="dd"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -424,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -443,14 +453,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +495,500 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[strata_fee_20230731.xlsx]pivot!PivotTable23</c:name>
+    <c:name>[strata_fee_20230731.xlsx]pivot!PivotTable1</c:name>
     <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivot!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>pivot!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>SIDDHARTH SINHA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>XIAOPENG FENG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DONGLI LIU</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TRACY CARRIER</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>EDWIN ALBERT IMHOFF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivot!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C2E5-4824-9E49-3C6FDE39A80B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1329728272"/>
+        <c:axId val="713974208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1329728272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="713974208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="713974208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1329728272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[strata_fee_20230731.xlsx]Sheet1!PivotTable23</c:name>
+    <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
@@ -888,6 +1393,120 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -900,7 +1519,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>pivot!$B$4</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -979,21 +1598,21 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>pivot!$A$5:$A$21</c:f>
+              <c:f>Sheet1!$A$5:$A$35</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>May</c:v>
+                    <c:v>Jun</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Jun</c:v>
+                    <c:v>Jul</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Jul</c:v>
+                    <c:v>Aug</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Aug</c:v>
+                    <c:v>Sep</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>Oct</c:v>
@@ -1014,16 +1633,60 @@
                     <c:v>Mar</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>May</c:v>
+                    <c:v>Apr</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Jun</c:v>
+                    <c:v>May</c:v>
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>Jul</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>Aug</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>02</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>02</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>02</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>02</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1039,7 +1702,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>pivot!$B$5:$B$21</c:f>
+              <c:f>Sheet1!$B$5:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1071,7 +1734,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -1090,7 +1753,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A979-4B72-B326-077941818D51}"/>
+              <c16:uniqueId val="{00000000-78F7-4A38-A95D-BB8B5D85646F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1309,498 +1972,6 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[strata_fee_20230731.xlsx]pivot!PivotTable1</c:name>
-    <c:fmtId val="0"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pivot!$B$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pivot!$A$25:$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>SIDDHARTH SINHA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>XIAOPENG FENG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>DONGLI LIU</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>TRACY CARRIER</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>EDWIN ALBERT IMHOFF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pivot!$B$25:$B$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C2E5-4824-9E49-3C6FDE39A80B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1329728272"/>
-        <c:axId val="713974208"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1329728272"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="713974208"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="713974208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1329728272"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2959,51 +3130,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A1FB961-C1CE-B923-44A8-D934A713B8AB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3023,7 +3158,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3033,13 +3168,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>89535</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3076,7 +3211,128 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8313420" y="4206240"/>
+              <a:off x="8313420" y="182880"/>
+              <a:ext cx="1828800" cy="2466975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E17E9D-2CBF-4AB7-8F3E-41DF96504FCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="payer 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{424E4201-3228-5E35-1528-F8C1DB64273C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="payer 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2697480" y="3040380"/>
               <a:ext cx="1828800" cy="2466975"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3601,7 +3857,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{915D806B-8927-47A8-8343-DEA578A58961}" name="PivotTable1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
-  <location ref="A24:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A2:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField numFmtId="15" showAll="0">
       <items count="48">
@@ -3739,10 +3995,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5709480-1479-4DD6-B514-8C458752D08E}" name="PivotTable23" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A4:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5709480-1479-4DD6-B514-8C458752D08E}" name="PivotTable23" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A4:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
-    <pivotField numFmtId="15" showAll="0">
+    <pivotField axis="axisRow" numFmtId="168" showAll="0">
       <items count="48">
         <item x="0"/>
         <item x="29"/>
@@ -3796,10 +4052,10 @@
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="6">
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
-        <item h="1" x="4"/>
+        <item x="4"/>
         <item h="1" x="1"/>
         <item t="default"/>
       </items>
@@ -3815,20 +4071,20 @@
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3853,57 +4109,100 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="3">
     <field x="5"/>
+    <field x="0"/>
     <field x="3"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="31">
     <i>
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
     </i>
     <i r="1">
       <x v="6"/>
     </i>
-    <i r="1">
+    <i r="2">
       <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
     </i>
     <i r="1">
       <x v="10"/>
     </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
     <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="2">
       <x v="11"/>
     </i>
     <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="2">
       <x v="12"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="2">
       <x v="1"/>
     </i>
     <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="2">
       <x v="2"/>
     </i>
     <i r="1">
+      <x v="30"/>
+    </i>
+    <i r="2">
       <x v="3"/>
     </i>
     <i r="1">
+      <x v="34"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="36"/>
+    </i>
+    <i r="2">
       <x v="5"/>
     </i>
     <i r="1">
-      <x v="6"/>
+      <x v="40"/>
     </i>
-    <i r="1">
+    <i r="2">
       <x v="7"/>
     </i>
     <i r="1">
+      <x v="43"/>
+    </i>
+    <i r="2">
       <x v="8"/>
     </i>
     <i t="grand">
@@ -3919,8 +4218,17 @@
   <dataFields count="1">
     <dataField name="Sum of fee_unit" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -3961,9 +4269,34 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_payer1" xr10:uid="{2054C292-E00F-40B0-A97F-8D0C8DCA2CAD}" sourceName="payer">
+  <pivotTables>
+    <pivotTable tabId="10" name="PivotTable23"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="2056893067">
+      <items count="5">
+        <i x="0"/>
+        <i x="1"/>
+        <i x="2"/>
+        <i x="3"/>
+        <i x="4" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
   <slicer name="payer" xr10:uid="{1D1F71E3-701E-4214-9249-E6BB59BF0CA4}" cache="Slicer_payer" caption="payer" rowHeight="234950"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="payer 1" xr10:uid="{3D2A6F61-D5D4-4E79-A93B-5AD4862FEC00}" cache="Slicer_payer1" caption="payer" rowHeight="234950"/>
 </slicers>
 </file>
 
@@ -4270,7 +4603,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -4287,7 +4620,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -4304,10 +4637,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4321,7 +4654,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -4338,7 +4671,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -4355,7 +4688,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -5476,8 +5809,8 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5499,7 +5832,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>44708</v>
       </c>
       <c r="B2" t="s">
@@ -5510,7 +5843,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>44741</v>
       </c>
       <c r="B3" t="s">
@@ -5521,7 +5854,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>44771</v>
       </c>
       <c r="B4" t="s">
@@ -5532,7 +5865,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>44804</v>
       </c>
       <c r="B5" t="s">
@@ -5543,7 +5876,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>44836</v>
       </c>
       <c r="B6" t="s">
@@ -5554,7 +5887,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>44866</v>
       </c>
       <c r="B7" t="s">
@@ -5565,7 +5898,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>44900</v>
       </c>
       <c r="B8" t="s">
@@ -5576,7 +5909,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>44927</v>
       </c>
       <c r="B9" t="s">
@@ -5587,7 +5920,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>44958</v>
       </c>
       <c r="B10" t="s">
@@ -5598,7 +5931,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>44987</v>
       </c>
       <c r="B11" t="s">
@@ -5609,7 +5942,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>45015</v>
       </c>
       <c r="B12" t="s">
@@ -5620,7 +5953,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>45047</v>
       </c>
       <c r="B13" t="s">
@@ -5631,7 +5964,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>45083</v>
       </c>
       <c r="B14" t="s">
@@ -5642,7 +5975,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>45112</v>
       </c>
       <c r="B15" t="s">
@@ -5653,7 +5986,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <v>45140</v>
       </c>
       <c r="B16" t="s">
@@ -5662,154 +5995,154 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>44715</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>44741</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>44773</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <v>44833</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <v>44866</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>44900</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <v>44958</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="9">
+      <c r="A24" s="8">
         <v>44987</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="9">
+      <c r="A25" s="8">
         <v>44987</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="9">
+      <c r="A26" s="8">
         <v>45016</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="9">
+      <c r="A27" s="8">
         <v>45047</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="9">
+      <c r="A28" s="8">
         <v>45111</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="9">
+      <c r="A29" s="8">
         <v>45138</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C29">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="9">
+      <c r="A30" s="8">
         <v>44715</v>
       </c>
       <c r="B30" t="s">
@@ -5820,7 +6153,7 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="9">
+      <c r="A31" s="8">
         <v>44742</v>
       </c>
       <c r="B31" t="s">
@@ -5831,7 +6164,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="9">
+      <c r="A32" s="8">
         <v>44774</v>
       </c>
       <c r="B32" t="s">
@@ -5842,7 +6175,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="9">
+      <c r="A33" s="8">
         <v>44813</v>
       </c>
       <c r="B33" t="s">
@@ -5853,7 +6186,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="9">
+      <c r="A34" s="8">
         <v>44838</v>
       </c>
       <c r="B34" t="s">
@@ -5864,7 +6197,7 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="9">
+      <c r="A35" s="8">
         <v>44879</v>
       </c>
       <c r="B35" t="s">
@@ -5875,7 +6208,7 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="9">
+      <c r="A36" s="8">
         <v>44922</v>
       </c>
       <c r="B36" t="s">
@@ -5886,7 +6219,7 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="9">
+      <c r="A37" s="8">
         <v>44922</v>
       </c>
       <c r="B37" t="s">
@@ -5897,7 +6230,7 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="9">
+      <c r="A38" s="8">
         <v>44981</v>
       </c>
       <c r="B38" t="s">
@@ -5908,7 +6241,7 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="9">
+      <c r="A39" s="8">
         <v>45047</v>
       </c>
       <c r="B39" t="s">
@@ -5919,7 +6252,7 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="9">
+      <c r="A40" s="8">
         <v>45047</v>
       </c>
       <c r="B40" t="s">
@@ -5930,7 +6263,7 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="9">
+      <c r="A41" s="8">
         <v>45047</v>
       </c>
       <c r="B41" t="s">
@@ -5941,7 +6274,7 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="9">
+      <c r="A42" s="8">
         <v>45133</v>
       </c>
       <c r="B42" t="s">
@@ -5950,10 +6283,10 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="E42" s="10"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="9">
+      <c r="A43" s="8">
         <v>45133</v>
       </c>
       <c r="B43" t="s">
@@ -5962,10 +6295,10 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="E43" s="10"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="9">
+      <c r="A44" s="8">
         <v>44712</v>
       </c>
       <c r="B44" t="s">
@@ -5976,7 +6309,7 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="9">
+      <c r="A45" s="8">
         <v>44743</v>
       </c>
       <c r="B45" t="s">
@@ -5987,7 +6320,7 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="9">
+      <c r="A46" s="8">
         <v>44772</v>
       </c>
       <c r="B46" t="s">
@@ -5998,7 +6331,7 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="9">
+      <c r="A47" s="8">
         <v>44805</v>
       </c>
       <c r="B47" t="s">
@@ -6009,7 +6342,7 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="9">
+      <c r="A48" s="8">
         <v>44834</v>
       </c>
       <c r="B48" t="s">
@@ -6020,7 +6353,7 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="9">
+      <c r="A49" s="8">
         <v>44862</v>
       </c>
       <c r="B49" t="s">
@@ -6031,7 +6364,7 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="9">
+      <c r="A50" s="8">
         <v>44896</v>
       </c>
       <c r="B50" t="s">
@@ -6042,7 +6375,7 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="9">
+      <c r="A51" s="8">
         <v>44926</v>
       </c>
       <c r="B51" t="s">
@@ -6053,7 +6386,7 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="9">
+      <c r="A52" s="8">
         <v>44957</v>
       </c>
       <c r="B52" t="s">
@@ -6064,7 +6397,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="9">
+      <c r="A53" s="8">
         <v>44986</v>
       </c>
       <c r="B53" t="s">
@@ -6075,7 +6408,7 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="9">
+      <c r="A54" s="8">
         <v>45016</v>
       </c>
       <c r="B54" t="s">
@@ -6086,7 +6419,7 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="9">
+      <c r="A55" s="8">
         <v>45044</v>
       </c>
       <c r="B55" t="s">
@@ -6097,7 +6430,7 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="9">
+      <c r="A56" s="8">
         <v>45076</v>
       </c>
       <c r="B56" t="s">
@@ -6108,7 +6441,7 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="9">
+      <c r="A57" s="8">
         <v>45107</v>
       </c>
       <c r="B57" t="s">
@@ -6119,7 +6452,7 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="9">
+      <c r="A58" s="8">
         <v>45135</v>
       </c>
       <c r="B58" t="s">
@@ -6128,10 +6461,10 @@
       <c r="C58">
         <v>1</v>
       </c>
-      <c r="E58" s="10"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="9">
+      <c r="A59" s="8">
         <v>44714</v>
       </c>
       <c r="B59" t="s">
@@ -6142,7 +6475,7 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="9">
+      <c r="A60" s="8">
         <v>44743</v>
       </c>
       <c r="B60" t="s">
@@ -6153,7 +6486,7 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="9">
+      <c r="A61" s="8">
         <v>44774</v>
       </c>
       <c r="B61" t="s">
@@ -6164,7 +6497,7 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="9">
+      <c r="A62" s="8">
         <v>44805</v>
       </c>
       <c r="B62" t="s">
@@ -6175,7 +6508,7 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="9">
+      <c r="A63" s="8">
         <v>44836</v>
       </c>
       <c r="B63" t="s">
@@ -6186,7 +6519,7 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="9">
+      <c r="A64" s="8">
         <v>44866</v>
       </c>
       <c r="B64" t="s">
@@ -6197,7 +6530,7 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="9">
+      <c r="A65" s="8">
         <v>44896</v>
       </c>
       <c r="B65" t="s">
@@ -6208,7 +6541,7 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="9">
+      <c r="A66" s="8">
         <v>44928</v>
       </c>
       <c r="B66" t="s">
@@ -6219,7 +6552,7 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="9">
+      <c r="A67" s="8">
         <v>44958</v>
       </c>
       <c r="B67" t="s">
@@ -6230,7 +6563,7 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="9">
+      <c r="A68" s="8">
         <v>44986</v>
       </c>
       <c r="B68" t="s">
@@ -6241,7 +6574,7 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="9">
+      <c r="A69" s="8">
         <v>45017</v>
       </c>
       <c r="B69" t="s">
@@ -6252,7 +6585,7 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="9">
+      <c r="A70" s="8">
         <v>45047</v>
       </c>
       <c r="B70" t="s">
@@ -6263,7 +6596,7 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="9">
+      <c r="A71" s="8">
         <v>45108</v>
       </c>
       <c r="B71" t="s">
@@ -6274,7 +6607,7 @@
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="9">
+      <c r="A72" s="8">
         <v>45140</v>
       </c>
       <c r="B72" t="s">
@@ -6283,7 +6616,7 @@
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="E72" s="10"/>
+      <c r="E72" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C66" xr:uid="{DC7BACAC-EFC0-4D7F-A488-F4B660678DD6}">
@@ -6301,10 +6634,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B089A-5F14-499D-895B-7DCA63C7442F}">
-  <dimension ref="A2:B30"/>
+  <dimension ref="A2:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6318,10 +6651,93 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="10">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF7185A-8110-455B-B2BC-16984DD5F5FC}">
+  <dimension ref="A2:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6336,201 +6752,257 @@
       <c r="A5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="12">
+        <v>44714</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12">
+        <v>44743</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12">
+        <v>44774</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12">
+        <v>44805</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="12">
+        <v>44836</v>
+      </c>
+      <c r="B14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="12">
+        <v>44866</v>
+      </c>
+      <c r="B16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12">
+        <v>44896</v>
+      </c>
+      <c r="B18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="12">
+        <v>44928</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="12">
+        <v>44958</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="12">
+        <v>44986</v>
+      </c>
+      <c r="B25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="12">
+        <v>45017</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="12">
+        <v>45047</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="8" t="s">
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="12">
+        <v>45108</v>
+      </c>
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="8" t="s">
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="12">
+        <v>45140</v>
+      </c>
+      <c r="B33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="7" t="s">
+      <c r="B34" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="11">
+      <c r="B35" s="10">
         <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="11">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="11">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
       <x14:slicerList>
-        <x14:slicer r:id="rId4"/>
+        <x14:slicer r:id="rId3"/>
       </x14:slicerList>
     </ext>
   </extLst>

</xml_diff>